<commit_message>
Fix misspelling in Excel
</commit_message>
<xml_diff>
--- a/Lab3_663380223-3.xlsx
+++ b/Lab3_663380223-3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario Summary" sheetId="1" r:id="rId1"/>
@@ -347,9 +347,6 @@
     <t>NullPointerException</t>
   </si>
   <si>
-    <t>No validation when input wrong format - not a roman numural</t>
-  </si>
-  <si>
     <t>No validation when input wrong format - wrong repeating digits</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>นายพิรัชย์ ชัยรัตน์ 663380223-3 Sec 1</t>
+  </si>
+  <si>
+    <t>No validation when input wrong format - not a roman numeral</t>
   </si>
 </sst>
 </file>
@@ -690,6 +690,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -748,12 +754,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1041,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -1107,7 +1107,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.65">
@@ -1155,32 +1155,32 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.65">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="3">
         <v>10</v>
       </c>
-      <c r="E8" s="55">
+      <c r="E8" s="35">
         <v>6</v>
       </c>
-      <c r="F8" s="56">
+      <c r="F8" s="36">
         <v>4</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.65">
-      <c r="A11" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
+      <c r="A11" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1268,29 +1268,29 @@
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.65">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
     </row>
     <row r="8" spans="1:7" ht="55.5" x14ac:dyDescent="0.65">
       <c r="A8" s="7" t="s">
@@ -1448,9 +1448,9 @@
       <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1491,14 +1491,14 @@
       <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12"/>
@@ -1512,39 +1512,39 @@
       <c r="A4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="51"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="51"/>
+      <c r="F5" s="53"/>
     </row>
     <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
     </row>
     <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="12"/>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -1595,7 +1595,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="46"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="11" t="s">
         <v>45</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="46"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="11" t="s">
         <v>72</v>
       </c>
@@ -1631,7 +1631,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="46"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="11" t="s">
         <v>73</v>
       </c>
@@ -1649,7 +1649,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="46"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="11" t="s">
         <v>76</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="46"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="11" t="s">
         <v>77</v>
       </c>
@@ -1685,7 +1685,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="46"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="11" t="s">
         <v>78</v>
       </c>
@@ -1703,7 +1703,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="46"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="11" t="s">
         <v>79</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="46"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="11" t="s">
         <v>80</v>
       </c>
@@ -1739,7 +1739,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="47"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="11" t="s">
         <v>81</v>
       </c>
@@ -1774,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="27.75" x14ac:dyDescent="0.65"/>
@@ -1847,7 +1847,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.65">
@@ -1872,7 +1872,7 @@
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.65">
@@ -1897,7 +1897,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="83.25" x14ac:dyDescent="0.65">
@@ -1922,7 +1922,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.65">
@@ -1933,7 +1933,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D7" s="21">
         <v>244325</v>
@@ -1947,7 +1947,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="83.25" x14ac:dyDescent="0.65">
@@ -1958,7 +1958,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="33">
         <v>244325</v>
@@ -1972,7 +1972,7 @@
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="83.25" x14ac:dyDescent="0.65">
@@ -1983,7 +1983,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="33">
         <v>244325</v>
@@ -1997,7 +1997,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>